<commit_message>
modified:   Analysis.xlsx 	modified:   MRhash_word.py - now the main MR file 	modified:   MasterSlave_chunkCorpus.py - timing 	modified:   MasterSlave_chunkMultCorpus.py - timing 	modified:   hashedfilenames.txt 	modified:   mpiRK_chunkCorpus.py - timing 	new file:   mpiRK_chunkMultCorpus.py - timing 	modified:   multipattern.txt 	modified:   regroupText.py 	new file:   regroupText2.py - main regroupText file 	new file:   ~$Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="8760"/>
+    <workbookView xWindow="7600" yWindow="0" windowWidth="18000" windowHeight="12580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Master-slave RKA</t>
   </si>
@@ -80,12 +85,51 @@
   <si>
     <t># of processors = 25</t>
   </si>
+  <si>
+    <t>Parallel Time code (Tp a )</t>
+  </si>
+  <si>
+    <t>Processing (tp b)</t>
+  </si>
+  <si>
+    <t>regroupText2.py Frankenstein X 20 40</t>
+  </si>
+  <si>
+    <t># processes</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t># chunks</t>
+  </si>
+  <si>
+    <t>mpiRK frankenstein</t>
+  </si>
+  <si>
+    <t>pat len</t>
+  </si>
+  <si>
+    <t>MasterSlave</t>
+  </si>
+  <si>
+    <t>time - parallel</t>
+  </si>
+  <si>
+    <t>preprocessing</t>
+  </si>
+  <si>
+    <t>Masterslave</t>
+  </si>
+  <si>
+    <t>at K = 4 processes, mpiRK works better than master/slave</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +141,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,14 +179,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -136,7 +228,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -160,11 +262,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -189,46 +294,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -240,50 +345,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.8144410957718291</c:v>
+                  <c:v>1.81444109577183</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2115689629625117</c:v>
+                  <c:v>3.211568962962512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9291218034948345</c:v>
+                  <c:v>4.929121803494834</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9175444501791468</c:v>
+                  <c:v>5.917544450179147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5062530260731615</c:v>
+                  <c:v>7.50625302607316</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4828435994274081</c:v>
+                  <c:v>8.482843599427408</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2115214916819301</c:v>
+                  <c:v>9.21152149168193</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>16.1574231331332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.305551217226636</c:v>
+                  <c:v>19.30555121722664</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19.85781326368113</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.190601142888823</c:v>
+                  <c:v>19.19060114288882</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.253030529014051</c:v>
+                  <c:v>19.25303052901405</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.087193757736689</c:v>
+                  <c:v>18.08719375773669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.457008232972713</c:v>
+                  <c:v>13.45700823297271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -309,46 +415,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,50 +466,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.90722054788591455</c:v>
+                  <c:v>0.907220547885915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0705229876541706</c:v>
+                  <c:v>1.070522987654171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2322804508737086</c:v>
+                  <c:v>1.232280450873709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1835088900358293</c:v>
+                  <c:v>1.183508890035829</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2510421710121935</c:v>
+                  <c:v>1.251042171012193</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2118347999182011</c:v>
+                  <c:v>1.211834799918201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1514401864602413</c:v>
+                  <c:v>1.151440186460241</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.009838945820825</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77222204868906541</c:v>
+                  <c:v>0.772222048689065</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5516059239911425</c:v>
+                  <c:v>0.551605923991142</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39164492128344536</c:v>
+                  <c:v>0.391644921283445</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.30082860201584455</c:v>
+                  <c:v>0.300828602015845</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.22329868836711961</c:v>
+                  <c:v>0.22329868836712</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.13457008232972714</c:v>
+                  <c:v>0.134570082329727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -429,46 +536,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,7 +587,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8122284000924673</c:v>
+                  <c:v>1.812228400092467</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.137807149253681</c:v>
@@ -489,17 +596,18 @@
                   <c:v>4.731018661972703</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.270028304003767</c:v>
+                  <c:v>5.270028304003766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2804022479267765</c:v>
+                  <c:v>6.280402247926776</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0428922362446844</c:v>
+                  <c:v>8.042892236244684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -525,46 +633,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -576,37 +684,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.90611420004623366</c:v>
+                  <c:v>0.906114200046234</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.379269049751227</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1827546654931758</c:v>
+                  <c:v>1.182754665493176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0540056608007533</c:v>
+                  <c:v>1.054005660800753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0467337079877961</c:v>
+                  <c:v>1.046733707987796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1489846051778121</c:v>
+                  <c:v>1.148984605177812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="105521920"/>
-        <c:axId val="105523456"/>
+        <c:smooth val="0"/>
+        <c:axId val="403986616"/>
+        <c:axId val="403992280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105521920"/>
+        <c:axId val="403986616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -625,26 +743,32 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105523456"/>
+        <c:crossAx val="403992280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105523456"/>
+        <c:axId val="403992280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105521920"/>
+        <c:crossAx val="403986616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -652,8 +776,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -665,7 +792,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -685,11 +822,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -714,46 +854,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,7 +905,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>30.520551000000001</c:v>
+                  <c:v>30.520551</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17.243205</c:v>
@@ -774,41 +914,42 @@
                   <c:v>11.234809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.3582300000000007</c:v>
+                  <c:v>9.35823</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.377548</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5282049999999998</c:v>
+                  <c:v>6.528205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0117909999999997</c:v>
+                  <c:v>6.011791</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.427387</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8684880000000001</c:v>
+                  <c:v>2.868488</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.788713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8856700000000002</c:v>
+                  <c:v>2.88567</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8763130000000001</c:v>
+                  <c:v>2.876313</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0617100000000002</c:v>
+                  <c:v>3.06171</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1151600000000004</c:v>
+                  <c:v>4.11516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -834,46 +975,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,60 +1026,71 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="83702912"/>
-        <c:axId val="83704832"/>
+        <c:smooth val="0"/>
+        <c:axId val="404055160"/>
+        <c:axId val="404060696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83702912"/>
+        <c:axId val="404055160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -957,26 +1109,32 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83704832"/>
+        <c:crossAx val="404060696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83704832"/>
+        <c:axId val="404060696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83702912"/>
+        <c:crossAx val="404055160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,12 +1142,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -997,7 +1158,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1021,11 +1192,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -1050,28 +1224,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1083,32 +1257,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>189.37070600000001</c:v>
+                  <c:v>189.370706</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128.65976800000001</c:v>
+                  <c:v>128.659768</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>112.393824</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.572889000000004</c:v>
+                  <c:v>90.572889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.175839999999994</c:v>
+                  <c:v>76.17583999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68.521719000000004</c:v>
+                  <c:v>68.521719</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.106879999999997</c:v>
+                  <c:v>60.10688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55.377741999999998</c:v>
+                  <c:v>55.377742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1134,28 +1309,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1167,10 +1342,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.7463740000000003</c:v>
+                  <c:v>5.746374</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9355260000000003</c:v>
+                  <c:v>4.935526</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.092384</c:v>
@@ -1179,31 +1354,41 @@
                   <c:v>3.499482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1534870000000002</c:v>
+                  <c:v>3.153487</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1606190000000001</c:v>
+                  <c:v>3.160619</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9825840000000001</c:v>
+                  <c:v>2.982584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8684880000000001</c:v>
+                  <c:v>2.868488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="83130624"/>
-        <c:axId val="83161088"/>
+        <c:smooth val="0"/>
+        <c:axId val="404096760"/>
+        <c:axId val="404102520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83130624"/>
+        <c:axId val="404096760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1227,21 +1412,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83161088"/>
+        <c:crossAx val="404102520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83161088"/>
+        <c:axId val="404102520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1261,10 +1450,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83130624"/>
+        <c:crossAx val="404096760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,12 +1464,494 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Time to complete constant work as processes,chunks increase</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Master/Slave</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$25:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$25:$M$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>mpiRK</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$25:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$25:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="464692552"/>
+        <c:axId val="464660408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="464692552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Processes (= Number of Chunks)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="464660408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="464660408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="464692552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.760723179667617"/>
+          <c:y val="0.384681102362205"/>
+          <c:w val="0.221923241156678"/>
+          <c:h val="0.296791641429437"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 Processes</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$D$35:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$35:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="465440040"/>
+        <c:axId val="423172088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="465440040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Chunks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="423172088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="423172088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="465440040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1370,6 +2044,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1662,17 +2401,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="7" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2273,31 +3012,577 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>410774</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>619621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>721655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1312159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>459929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>660568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(4.88, 4.77)</f>
+        <v>4.8249999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(5.03, 5.36)</f>
+        <v>5.1950000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>128</v>
+      </c>
+      <c r="D19">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>256</v>
+      </c>
+      <c r="D20">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>179</v>
+      </c>
+      <c r="F25">
+        <v>2.96</v>
+      </c>
+      <c r="G25">
+        <v>5.19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>20</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>6.21</v>
+      </c>
+      <c r="N25">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>179</v>
+      </c>
+      <c r="F26">
+        <v>2.48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>179</v>
+      </c>
+      <c r="F27">
+        <v>1.52</v>
+      </c>
+      <c r="G27">
+        <v>5.19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <v>8</v>
+      </c>
+      <c r="M27">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>179</v>
+      </c>
+      <c r="F28">
+        <v>0.77</v>
+      </c>
+      <c r="I28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28">
+        <v>16</v>
+      </c>
+      <c r="L28">
+        <v>16</v>
+      </c>
+      <c r="M28">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="F29">
+        <v>0.41</v>
+      </c>
+      <c r="I29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29">
+        <v>32</v>
+      </c>
+      <c r="L29">
+        <v>32</v>
+      </c>
+      <c r="M29">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>64</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30">
+        <v>64</v>
+      </c>
+      <c r="L30">
+        <v>64</v>
+      </c>
+      <c r="M30">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>128</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>0.16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31">
+        <v>128</v>
+      </c>
+      <c r="L31">
+        <v>128</v>
+      </c>
+      <c r="M31">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>179</v>
+      </c>
+      <c r="F35">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>4.87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="F39">
+        <v>4.4800000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>128</v>
+      </c>
+      <c r="F41">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>256</v>
+      </c>
+      <c r="F42">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>